<commit_message>
(2020-06-16) book_cnt, ans.html 작성 중.
</commit_message>
<xml_diff>
--- a/Documents/정책정의서.xlsx
+++ b/Documents/정책정의서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Publisher_Portfolio\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2696EC69-B3E5-40C2-9541-C635486FDF45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1146FB6-75B3-47C5-907C-782048CB45B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="표지" sheetId="3" r:id="rId1"/>
@@ -971,123 +971,123 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1164,12 +1164,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1186,6 +1180,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1806,7 +1806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F001FD6C-242E-4ABF-B23F-99121D6A9B9C}">
   <dimension ref="B1:S33"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="X31" sqref="X31"/>
     </sheetView>
   </sheetViews>
@@ -2085,18 +2085,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="24" customWidth="1"/>
-    <col min="2" max="7" width="8.75" style="24"/>
-    <col min="8" max="8" width="18.75" style="24" customWidth="1"/>
-    <col min="9" max="9" width="8.75" style="24"/>
-    <col min="10" max="12" width="12" style="24" customWidth="1"/>
-    <col min="13" max="14" width="8.75" style="24"/>
-    <col min="15" max="15" width="3.25" style="24" customWidth="1"/>
-    <col min="16" max="16" width="18.75" style="24" customWidth="1"/>
-    <col min="17" max="18" width="11.25" style="24" customWidth="1"/>
-    <col min="19" max="21" width="14" style="24" customWidth="1"/>
-    <col min="22" max="22" width="1.625" style="24" customWidth="1"/>
-    <col min="23" max="16384" width="8.75" style="24"/>
+    <col min="1" max="1" width="1.625" style="20" customWidth="1"/>
+    <col min="2" max="7" width="8.75" style="20"/>
+    <col min="8" max="8" width="18.75" style="20" customWidth="1"/>
+    <col min="9" max="9" width="8.75" style="20"/>
+    <col min="10" max="12" width="12" style="20" customWidth="1"/>
+    <col min="13" max="14" width="8.75" style="20"/>
+    <col min="15" max="15" width="3.25" style="20" customWidth="1"/>
+    <col min="16" max="16" width="18.75" style="20" customWidth="1"/>
+    <col min="17" max="18" width="11.25" style="20" customWidth="1"/>
+    <col min="19" max="21" width="14" style="20" customWidth="1"/>
+    <col min="22" max="22" width="1.625" style="20" customWidth="1"/>
+    <col min="23" max="16384" width="8.75" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2302,7 +2302,7 @@
         <v>66</v>
       </c>
       <c r="N10" s="67"/>
-      <c r="P10" s="25" t="s">
+      <c r="P10" s="21" t="s">
         <v>67</v>
       </c>
       <c r="Q10" s="68" t="s">
@@ -2316,488 +2316,488 @@
       <c r="U10" s="69"/>
     </row>
     <row r="11" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="44">
+      <c r="B11" s="47">
         <v>0.1</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46">
+      <c r="C11" s="48"/>
+      <c r="D11" s="54">
         <v>43964</v>
       </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="53" t="s">
+      <c r="E11" s="48"/>
+      <c r="F11" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="45" t="s">
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="N11" s="47"/>
-      <c r="P11" s="18" t="s">
+      <c r="N11" s="50"/>
+      <c r="P11" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="Q11" s="53" t="s">
+      <c r="Q11" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="R11" s="53"/>
-      <c r="S11" s="53" t="s">
+      <c r="R11" s="49"/>
+      <c r="S11" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="T11" s="53"/>
-      <c r="U11" s="54"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="51"/>
     </row>
     <row r="12" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="44">
+      <c r="B12" s="47">
         <v>0.2</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="46">
+      <c r="C12" s="48"/>
+      <c r="D12" s="54">
         <v>43967</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="53" t="s">
+      <c r="E12" s="54"/>
+      <c r="F12" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="45" t="s">
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="N12" s="47"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="53"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="54"/>
+      <c r="N12" s="50"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="51"/>
     </row>
     <row r="13" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="47"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="53"/>
-      <c r="R13" s="53"/>
-      <c r="S13" s="53"/>
-      <c r="T13" s="53"/>
-      <c r="U13" s="54"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="50"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
+      <c r="U13" s="51"/>
     </row>
     <row r="14" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="47"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="53"/>
-      <c r="R14" s="53"/>
-      <c r="S14" s="53"/>
-      <c r="T14" s="53"/>
-      <c r="U14" s="54"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="50"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="49"/>
+      <c r="U14" s="51"/>
     </row>
     <row r="15" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="47"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="53"/>
-      <c r="R15" s="53"/>
-      <c r="S15" s="53"/>
-      <c r="T15" s="53"/>
-      <c r="U15" s="54"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="50"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="51"/>
     </row>
     <row r="16" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="47"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="53"/>
-      <c r="R16" s="53"/>
-      <c r="S16" s="53"/>
-      <c r="T16" s="53"/>
-      <c r="U16" s="54"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="50"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
+      <c r="U16" s="51"/>
     </row>
     <row r="17" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="47"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="53"/>
-      <c r="T17" s="53"/>
-      <c r="U17" s="54"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="50"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+      <c r="U17" s="51"/>
     </row>
     <row r="18" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="47"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="53"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="54"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="50"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="51"/>
     </row>
     <row r="19" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="47"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="53"/>
-      <c r="T19" s="53"/>
-      <c r="U19" s="54"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="50"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="49"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="51"/>
     </row>
     <row r="20" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="47"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="53"/>
-      <c r="S20" s="53"/>
-      <c r="T20" s="53"/>
-      <c r="U20" s="54"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="50"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+      <c r="U20" s="51"/>
     </row>
     <row r="21" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="47"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="45"/>
-      <c r="S21" s="53"/>
-      <c r="T21" s="53"/>
-      <c r="U21" s="54"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="50"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+      <c r="U21" s="51"/>
     </row>
     <row r="22" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="47"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="45"/>
-      <c r="S22" s="53"/>
-      <c r="T22" s="53"/>
-      <c r="U22" s="54"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="50"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="49"/>
+      <c r="T22" s="49"/>
+      <c r="U22" s="51"/>
     </row>
     <row r="23" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="47"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="45"/>
-      <c r="S23" s="53"/>
-      <c r="T23" s="53"/>
-      <c r="U23" s="54"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="50"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="49"/>
+      <c r="U23" s="51"/>
     </row>
     <row r="24" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="44"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="47"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="45"/>
-      <c r="R24" s="45"/>
-      <c r="S24" s="53"/>
-      <c r="T24" s="53"/>
-      <c r="U24" s="54"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="50"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="48"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="49"/>
+      <c r="U24" s="51"/>
     </row>
     <row r="25" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="47"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="45"/>
-      <c r="R25" s="45"/>
-      <c r="S25" s="53"/>
-      <c r="T25" s="53"/>
-      <c r="U25" s="54"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="50"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="48"/>
+      <c r="R25" s="48"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="49"/>
+      <c r="U25" s="51"/>
     </row>
     <row r="26" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="44"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="47"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="53"/>
-      <c r="T26" s="53"/>
-      <c r="U26" s="54"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="50"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="48"/>
+      <c r="R26" s="48"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="49"/>
+      <c r="U26" s="51"/>
     </row>
     <row r="27" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="44"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="47"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="45"/>
-      <c r="R27" s="45"/>
-      <c r="S27" s="53"/>
-      <c r="T27" s="53"/>
-      <c r="U27" s="54"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="50"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="48"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="49"/>
+      <c r="U27" s="51"/>
     </row>
     <row r="28" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="44"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="47"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="53"/>
-      <c r="T28" s="53"/>
-      <c r="U28" s="54"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="50"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="48"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="49"/>
+      <c r="U28" s="51"/>
     </row>
     <row r="29" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="44"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="47"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="53"/>
-      <c r="T29" s="53"/>
-      <c r="U29" s="54"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="50"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="48"/>
+      <c r="R29" s="48"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="49"/>
+      <c r="U29" s="51"/>
     </row>
     <row r="30" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="44"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="47"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="53"/>
-      <c r="T30" s="53"/>
-      <c r="U30" s="54"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="50"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="48"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="49"/>
+      <c r="U30" s="51"/>
     </row>
     <row r="31" spans="2:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="44"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="47"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
-      <c r="S31" s="53"/>
-      <c r="T31" s="53"/>
-      <c r="U31" s="54"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="50"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="49"/>
+      <c r="U31" s="51"/>
     </row>
     <row r="32" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="48"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="50"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="51"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="49"/>
-      <c r="S32" s="50"/>
-      <c r="T32" s="50"/>
-      <c r="U32" s="52"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="53"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="44"/>
+      <c r="R32" s="44"/>
+      <c r="S32" s="45"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="152">
@@ -2840,6 +2840,11 @@
     <mergeCell ref="Q13:R13"/>
     <mergeCell ref="S13:U13"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="F16:L16"/>
@@ -2873,6 +2878,9 @@
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="S19:U19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:L20"/>
     <mergeCell ref="Q23:R23"/>
     <mergeCell ref="S23:U23"/>
     <mergeCell ref="B22:C22"/>
@@ -2887,6 +2895,10 @@
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="Q21:R21"/>
     <mergeCell ref="S21:U21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:L23"/>
+    <mergeCell ref="M23:N23"/>
     <mergeCell ref="Q26:R26"/>
     <mergeCell ref="S26:U26"/>
     <mergeCell ref="B25:C25"/>
@@ -2901,6 +2913,10 @@
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="Q24:R24"/>
     <mergeCell ref="S24:U24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:L26"/>
+    <mergeCell ref="M26:N26"/>
     <mergeCell ref="Q29:R29"/>
     <mergeCell ref="S29:U29"/>
     <mergeCell ref="B28:C28"/>
@@ -2915,6 +2931,10 @@
     <mergeCell ref="M27:N27"/>
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="S27:U27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:L29"/>
+    <mergeCell ref="M29:N29"/>
     <mergeCell ref="Q32:R32"/>
     <mergeCell ref="S32:U32"/>
     <mergeCell ref="B31:C31"/>
@@ -2929,30 +2949,10 @@
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="Q30:R30"/>
     <mergeCell ref="S30:U30"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="F32:L32"/>
     <mergeCell ref="M32:N32"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:L20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2965,7 +2965,7 @@
   <dimension ref="B1:G7"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3001,7 +3001,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -3016,12 +3016,12 @@
       <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="22" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -3036,12 +3036,12 @@
       <c r="F4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -3056,12 +3056,12 @@
       <c r="F5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -3076,18 +3076,18 @@
       <c r="F6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="21">
+      <c r="B7" s="18">
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="19" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="15" t="s">
@@ -3096,7 +3096,7 @@
       <c r="F7" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="25" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3111,8 +3111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3161,16 +3161,16 @@
       </c>
     </row>
     <row r="3" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="82">
+      <c r="B3" s="87">
         <v>1</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="81" t="s">
+      <c r="E3" s="86" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -3188,15 +3188,15 @@
       <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="83" t="s">
+      <c r="K3" s="81" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
@@ -3212,13 +3212,13 @@
       <c r="J4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="84"/>
+      <c r="K4" s="82"/>
     </row>
     <row r="5" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
@@ -3234,19 +3234,19 @@
       <c r="J5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="85"/>
+      <c r="K5" s="83"/>
     </row>
     <row r="6" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="44">
+      <c r="B6" s="47">
         <v>2</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="48" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -3264,15 +3264,15 @@
       <c r="J6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="86" t="s">
+      <c r="K6" s="84" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
@@ -3288,13 +3288,13 @@
       <c r="J7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="84"/>
+      <c r="K7" s="82"/>
     </row>
     <row r="8" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
       <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
@@ -3310,19 +3310,19 @@
       <c r="J8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="85"/>
+      <c r="K8" s="83"/>
     </row>
     <row r="9" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="44">
+      <c r="B9" s="47">
         <v>3</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="48" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -3340,15 +3340,15 @@
       <c r="J9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="86" t="s">
+      <c r="K9" s="84" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="3" t="s">
         <v>14</v>
       </c>
@@ -3364,13 +3364,13 @@
       <c r="J10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="84"/>
+      <c r="K10" s="82"/>
     </row>
     <row r="11" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="3" t="s">
         <v>15</v>
       </c>
@@ -3386,19 +3386,19 @@
       <c r="J11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="85"/>
+      <c r="K11" s="83"/>
     </row>
     <row r="12" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="44">
+      <c r="B12" s="47">
         <v>4</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="48" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -3416,15 +3416,15 @@
       <c r="J12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="84" t="s">
+      <c r="K12" s="82" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="3" t="s">
         <v>14</v>
       </c>
@@ -3440,13 +3440,13 @@
       <c r="J13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="84"/>
+      <c r="K13" s="82"/>
     </row>
     <row r="14" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
       <c r="F14" s="3" t="s">
         <v>15</v>
       </c>
@@ -3462,19 +3462,19 @@
       <c r="J14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="85"/>
+      <c r="K14" s="83"/>
     </row>
     <row r="15" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="44">
+      <c r="B15" s="47">
         <v>5</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="48" t="s">
         <v>53</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -3492,15 +3492,15 @@
       <c r="J15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="86" t="s">
+      <c r="K15" s="84" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
       <c r="F16" s="3" t="s">
         <v>14</v>
       </c>
@@ -3516,13 +3516,13 @@
       <c r="J16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="84"/>
+      <c r="K16" s="82"/>
     </row>
     <row r="17" spans="2:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="15" t="s">
         <v>15</v>
       </c>
@@ -3538,7 +3538,7 @@
       <c r="J17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="87"/>
+      <c r="K17" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="25">

</xml_diff>